<commit_message>
Modifications to graphs, editing observed data file errors
</commit_message>
<xml_diff>
--- a/Prototypes/Canola/GenomicsPhenology.xlsx
+++ b/Prototypes/Canola/GenomicsPhenology.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lil026\ApsimX\Prototypes\Canola\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5AF3975-8263-4348-A1F2-B556E6F03E37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38178A8E-C11E-4321-BD50-C9D06BE6CE62}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{2EF320CE-7ABE-42F3-AF68-7A3FE40785D1}"/>
+    <workbookView xWindow="0" yWindow="360" windowWidth="38640" windowHeight="21240" xr2:uid="{2EF320CE-7ABE-42F3-AF68-7A3FE40785D1}"/>
   </bookViews>
   <sheets>
     <sheet name="OBSPhenology" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">OBSLeafAppearance!$A$1:$L$631</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">OBSPhenology!$A$1:$N$106</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4366" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4368" uniqueCount="143">
   <si>
     <t>SimulationName</t>
   </si>
@@ -462,6 +463,12 @@
   <si>
     <t>York2020TOS20-MayCvATR_Gem</t>
   </si>
+  <si>
+    <t>Exclude</t>
+  </si>
+  <si>
+    <t>junk</t>
+  </si>
 </sst>
 </file>
 
@@ -813,10 +820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C14EF01D-4333-43EA-8852-85C5FAA2F335}">
-  <dimension ref="A1:M106"/>
+  <dimension ref="A1:N106"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I119" sqref="I119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,7 +843,7 @@
     <col min="13" max="13" width="35.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -876,8 +883,11 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -917,8 +927,11 @@
       <c r="M2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -959,7 +972,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -1000,7 +1013,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>115</v>
       </c>
@@ -1019,9 +1032,6 @@
       <c r="F5">
         <v>116</v>
       </c>
-      <c r="G5">
-        <v>148</v>
-      </c>
       <c r="H5">
         <v>28</v>
       </c>
@@ -1040,8 +1050,11 @@
       <c r="M5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>117</v>
       </c>
@@ -1082,7 +1095,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>118</v>
       </c>
@@ -1123,7 +1136,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>128</v>
       </c>
@@ -1163,8 +1176,11 @@
       <c r="M8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>130</v>
       </c>
@@ -1205,7 +1221,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>131</v>
       </c>
@@ -1246,7 +1262,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1287,7 +1303,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1328,7 +1344,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1368,8 +1384,11 @@
       <c r="M13" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1410,7 +1429,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1451,7 +1470,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1492,7 +1511,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1533,7 +1552,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1552,9 +1571,6 @@
       <c r="F18">
         <v>95</v>
       </c>
-      <c r="G18">
-        <v>137</v>
-      </c>
       <c r="H18">
         <v>28</v>
       </c>
@@ -1573,8 +1589,11 @@
       <c r="M18" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1593,9 +1612,6 @@
       <c r="F19">
         <v>68</v>
       </c>
-      <c r="G19">
-        <v>99</v>
-      </c>
       <c r="H19">
         <v>28</v>
       </c>
@@ -1614,8 +1630,11 @@
       <c r="M19" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -1656,7 +1675,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -1697,7 +1716,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -1716,9 +1735,6 @@
       <c r="F22">
         <v>60</v>
       </c>
-      <c r="G22">
-        <v>148</v>
-      </c>
       <c r="H22">
         <v>28</v>
       </c>
@@ -1737,8 +1753,11 @@
       <c r="M22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -1779,7 +1798,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -1820,7 +1839,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -1861,7 +1880,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -1902,7 +1921,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>119</v>
       </c>
@@ -1943,7 +1962,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>120</v>
       </c>
@@ -1984,7 +2003,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>132</v>
       </c>
@@ -2025,7 +2044,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>133</v>
       </c>
@@ -2066,7 +2085,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -2085,9 +2104,6 @@
       <c r="F31">
         <v>56</v>
       </c>
-      <c r="G31">
-        <v>74</v>
-      </c>
       <c r="H31">
         <v>17</v>
       </c>
@@ -2106,8 +2122,11 @@
       <c r="M31" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N31">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -2126,9 +2145,6 @@
       <c r="F32">
         <v>68</v>
       </c>
-      <c r="G32">
-        <v>78</v>
-      </c>
       <c r="H32">
         <v>14</v>
       </c>
@@ -2146,6 +2162,9 @@
       </c>
       <c r="M32" t="s">
         <v>19</v>
+      </c>
+      <c r="N32">
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -5183,16 +5202,17 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:N106" xr:uid="{BCFA0856-B878-4A28-B408-F40C8F5EA065}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B5B9EA-70C2-4333-AA33-B5A6A85DE8B6}">
-  <dimension ref="A1:L602"/>
+  <dimension ref="A1:M602"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L816"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5202,7 +5222,7 @@
     <col min="10" max="10" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5239,8 +5259,11 @@
       <c r="L1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -5278,7 +5301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -5316,7 +5339,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -5354,7 +5377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -5392,7 +5415,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -5430,7 +5453,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -5468,7 +5491,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -5506,7 +5529,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -5544,7 +5567,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -5582,7 +5605,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -5620,7 +5643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -5658,7 +5681,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -5696,7 +5719,7 @@
         <v>2.57</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -5734,7 +5757,7 @@
         <v>3.62</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -5772,7 +5795,7 @@
         <v>4.88</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>

</xml_diff>